<commit_message>
LAB 18 + ConvertExcel2Json
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data/ValidCredExcel.xlsx
+++ b/src/main/resources/test-data/ValidCredExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/maven-appium-k5/src/main/resources/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E52684E-2AE0-6542-9ADF-3CBE974E0BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB45210-F550-3045-B4F7-7FD58E0BCD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16320" xr2:uid="{02451B66-7C78-5A47-977E-6F81CDB7CB0C}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{02451B66-7C78-5A47-977E-6F81CDB7CB0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -44,6 +44,24 @@
   </si>
   <si>
     <t>user2@gmail.com</t>
+  </si>
+  <si>
+    <t>a12345678</t>
+  </si>
+  <si>
+    <t>876543s21</t>
+  </si>
+  <si>
+    <t>khoa01@gg.vn</t>
+  </si>
+  <si>
+    <t>abc123413</t>
+  </si>
+  <si>
+    <t>khoa99@gj.sd</t>
+  </si>
+  <si>
+    <t>13jfsfsj323</t>
   </si>
 </sst>
 </file>
@@ -406,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BDAE74-A8F1-BE42-862E-618260DAE70C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,22 +447,40 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>12345678</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>87654321</v>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{2EC733FB-5BF3-1946-9702-33BAAD54B80A}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{3188CFA9-CB12-AC4D-9F57-1B41DB8722F0}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{44C25C8F-D41A-844E-B727-9D2917D46727}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{FEA80A59-45CA-164A-9084-E087AC031CCE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>